<commit_message>
Examples 22 to 24 added
</commit_message>
<xml_diff>
--- a/AMC_examples_data/AMC_examples_data_ex11.xlsx
+++ b/AMC_examples_data/AMC_examples_data_ex11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\AMC_examples_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B7AEC5-9AB9-4E7D-AEEF-AA35065D98BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B889F59A-7C60-4EF6-9290-04B036F377A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>frame_h</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>comp_offs_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -458,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F28914-79CE-4C5A-92B2-E41C9BEF8F7E}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +579,7 @@
         <v>19</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2">
         <v>12</v>
@@ -641,6 +644,27 @@
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>40</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>44</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>48</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>